<commit_message>
original code, new algorithm and matrices.xlsx updated
</commit_message>
<xml_diff>
--- a/matrices.xlsx
+++ b/matrices.xlsx
@@ -1,59 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akaha\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10245658-817A-4F93-A795-305AF9E2B31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E62A09B-9860-4266-A439-6DD093DDF108}"/>
+    <workbookView windowWidth="23220" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Group/Name</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>DOP (degree of parallelism)</t>
+  </si>
+  <si>
+    <t># of levels</t>
+  </si>
   <si>
     <t>VanVelzen/Zd_Jac2_db</t>
   </si>
   <si>
+    <t>Chemical Process Simulation Problem</t>
+  </si>
+  <si>
     <t>HVDC/hvdc2</t>
   </si>
   <si>
+    <t>Power Network Problem</t>
+  </si>
+  <si>
     <t>HB/bcsstk17</t>
   </si>
   <si>
     <t>Structural Problem</t>
   </si>
   <si>
-    <t>Power Network Problem</t>
-  </si>
-  <si>
-    <t>Chemical Process Simulation Problem</t>
-  </si>
-  <si>
     <t>Simon/venkat01</t>
   </si>
   <si>
@@ -87,12 +82,6 @@
     <t>Directed Weighted Graph</t>
   </si>
   <si>
-    <t>DOP</t>
-  </si>
-  <si>
-    <t># of levels</t>
-  </si>
-  <si>
     <t>Schenk_ISEI/barrier2-12</t>
   </si>
   <si>
@@ -108,29 +97,180 @@
     <t>Computational Fluid Dynamics Problem</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Group/Name</t>
-  </si>
-  <si>
-    <t>Kind</t>
+    <t>SuiteSparse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +289,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -158,27 +484,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -227,7 +839,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -260,26 +872,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -312,23 +907,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,7 +914,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -360,9 +938,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -386,7 +964,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -439,7 +1017,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -464,94 +1042,91 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1B4FF9-B790-4034-9382-D9E7460A3804}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="25.90625" customWidth="1"/>
-    <col min="3" max="3" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.9037037037037" customWidth="true"/>
+    <col min="3" max="3" width="41.5407407407407" customWidth="true"/>
+    <col min="4" max="4" width="27.6666666666667" customWidth="true"/>
+    <col min="5" max="5" width="12.7777777777778" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1337</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1875</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>820</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>14.99</v>
@@ -560,15 +1135,15 @@
         <v>4176</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>971</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>22.39</v>
@@ -577,15 +1152,15 @@
         <v>7760</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>1362</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>1.01</v>
@@ -594,15 +1169,15 @@
         <v>181783</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1580</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>98.02</v>
@@ -611,32 +1186,32 @@
         <v>6765</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>1418</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
-        <v>1164.4000000000001</v>
+        <v>1164.4</v>
       </c>
       <c r="E9">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>914</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>35</v>
@@ -645,15 +1220,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>963</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>84.23</v>
@@ -662,15 +1237,15 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>1254</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>227.21</v>
@@ -679,22 +1254,28 @@
         <v>729</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>894</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>478</v>
       </c>
     </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>